<commit_message>
Added filtering options for services
api endpoint list also updated
</commit_message>
<xml_diff>
--- a/API_endpoint_list.xlsx
+++ b/API_endpoint_list.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Technikus\Documents\GitHub\HandyGo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Munka\13C_info2\HandyGo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C16EE1F-E3ED-4C04-BB46-610A3D064943}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4F27FF2-F7A6-4716-A862-3FAFCF74F14C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E0E4588E-4664-4B85-8DE9-D10EECA0DBCE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E0E4588E-4664-4B85-8DE9-D10EECA0DBCE}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="70">
   <si>
     <t>API elérési út</t>
   </si>
@@ -48,9 +48,6 @@
     <t>body adatok</t>
   </si>
   <si>
-    <t>header adatok</t>
-  </si>
-  <si>
     <t>auth/login</t>
   </si>
   <si>
@@ -238,6 +235,18 @@
   </si>
   <si>
     <t>Az admin regisztráció csak admin bejelentkezés után működik</t>
+  </si>
+  <si>
+    <t>Szolgáltatás szűrése távolság alapján</t>
+  </si>
+  <si>
+    <t>paraméter adatok</t>
+  </si>
+  <si>
+    <t>service/:lat/:lon</t>
+  </si>
+  <si>
+    <t>szélesség, hosszúság</t>
   </si>
 </sst>
 </file>
@@ -280,7 +289,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -448,18 +457,61 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -472,7 +524,35 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -484,105 +564,84 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thick">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="thick">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thick">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -591,7 +650,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -604,21 +663,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -933,10 +995,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2337CF4-35BF-4E47-9BF9-5BAF47D2C70E}">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -945,386 +1007,401 @@
     <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="41.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" s="14" t="s">
+      <c r="B1" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="15" t="s">
-        <v>3</v>
+      <c r="E1" s="14" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="D2" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E2" s="10"/>
-      <c r="G2" s="16" t="s">
-        <v>50</v>
+      <c r="G2" s="15" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>7</v>
-      </c>
       <c r="D3" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E3" s="8"/>
-      <c r="G3" s="16" t="s">
-        <v>65</v>
+      <c r="G3" s="15" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="16" t="s">
-        <v>66</v>
+        <v>10</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="E5" s="6"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="6"/>
     </row>
     <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="E8" s="10"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" s="10"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="6"/>
+      <c r="C9" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="10" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>24</v>
+        <v>47</v>
       </c>
       <c r="D10" s="1"/>
-      <c r="E10" s="6" t="s">
-        <v>11</v>
-      </c>
+      <c r="E10" s="6"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>17</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="D11" s="1"/>
       <c r="E11" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C12" s="1" t="s">
+      <c r="B14" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="7" t="s">
+      <c r="D14" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D13" s="4" t="s">
+      <c r="B15" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E13" s="8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C14" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E14" s="10"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D15" s="1"/>
-      <c r="E15" s="6" t="s">
-        <v>11</v>
-      </c>
+      <c r="E15" s="10"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D16" s="1"/>
-      <c r="E16" s="6"/>
+      <c r="E16" s="6" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="6"/>
     </row>
-    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="C18" s="17" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="1"/>
+      <c r="E18" s="6"/>
+    </row>
+    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="17" t="s">
+      <c r="E19" s="17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="E18" s="18" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="21" t="s">
+      <c r="C20" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="D20" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="E20" s="20"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="B19" s="22" t="s">
+      <c r="B21" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="D21" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="E21" s="6"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="C19" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="D19" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="E19" s="23"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="B20" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="C20" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="D20" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E20" s="6"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="B21" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="C21" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="D21" s="1"/>
-      <c r="E21" s="6"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="B22" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="C22" s="19" t="s">
-        <v>58</v>
+      <c r="C22" s="18" t="s">
+        <v>47</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="6"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="21" t="s">
-        <v>55</v>
+      <c r="A23" s="28" t="s">
+        <v>53</v>
       </c>
       <c r="B23" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="19" t="s">
-        <v>59</v>
+      <c r="C23" s="18" t="s">
+        <v>57</v>
       </c>
       <c r="D23" s="1"/>
-      <c r="E23" s="6" t="s">
-        <v>11</v>
-      </c>
+      <c r="E23" s="6"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>60</v>
+      <c r="A24" s="28" t="s">
+        <v>54</v>
       </c>
       <c r="B24" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="C24" s="19" t="s">
-        <v>62</v>
+        <v>43</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>58</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="B25" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="C25" s="26" t="s">
-        <v>63</v>
-      </c>
-      <c r="D25" s="3"/>
-      <c r="E25" s="12"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="B26" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="D26" s="3"/>
+      <c r="E26" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add 'My Services' feature for service providers
Implemented backend and frontend support for users to view their own services. Added a new API endpoint and controller method to fetch services by worker ID, updated Angular routing and navigation, and created a new MyServicesComponent to display the user's services. Also improved booking logic to prevent duplicate bookings and enhanced service detail and booking flows.
</commit_message>
<xml_diff>
--- a/API_endpoint_list.xlsx
+++ b/API_endpoint_list.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Munka\13C_info2\HandyGo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Technikus\Documents\GitHub\HandyGo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4F27FF2-F7A6-4716-A862-3FAFCF74F14C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EABEF09-69A2-4D12-8CDC-0B2A46BBD25F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E0E4588E-4664-4B85-8DE9-D10EECA0DBCE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E0E4588E-4664-4B85-8DE9-D10EECA0DBCE}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="72">
   <si>
     <t>API elérési út</t>
   </si>
@@ -247,6 +247,12 @@
   </si>
   <si>
     <t>szélesség, hosszúság</t>
+  </si>
+  <si>
+    <t>service/my-services</t>
+  </si>
+  <si>
+    <t>A felhasználó szolgáltatásainak lekérése</t>
   </si>
 </sst>
 </file>
@@ -995,10 +1001,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2337CF4-35BF-4E47-9BF9-5BAF47D2C70E}">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1214,194 +1220,207 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="7" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="D14" s="16"/>
+      <c r="E14" s="17"/>
+    </row>
+    <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B15" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C15" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D15" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E14" s="8" t="s">
+      <c r="E15" s="8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
+    <row r="16" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B16" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E15" s="10"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D16" s="1"/>
-      <c r="E16" s="6" t="s">
-        <v>10</v>
-      </c>
+      <c r="E16" s="10"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D17" s="1"/>
-      <c r="E17" s="6"/>
+      <c r="E17" s="6" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="6"/>
     </row>
-    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="26" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" s="1"/>
+      <c r="E19" s="6"/>
+    </row>
+    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="16" t="s">
+      <c r="B20" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="C19" s="16" t="s">
+      <c r="C20" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="D19" s="16" t="s">
+      <c r="D20" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="E19" s="17" t="s">
+      <c r="E20" s="17" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="27" t="s">
+    <row r="21" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="B20" s="23" t="s">
+      <c r="B21" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="19" t="s">
+      <c r="C21" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="D20" s="19" t="s">
+      <c r="D21" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="E20" s="20"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="B21" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="C21" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="D21" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="E21" s="6"/>
+      <c r="E21" s="20"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="28" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B22" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="D22" s="1"/>
+        <v>56</v>
+      </c>
+      <c r="D22" s="18" t="s">
+        <v>63</v>
+      </c>
       <c r="E22" s="6"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B23" s="24" t="s">
         <v>44</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="6"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="D24" s="1"/>
+      <c r="E24" s="6"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="28" t="s">
         <v>54</v>
-      </c>
-      <c r="B24" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="C24" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="D24" s="1"/>
-      <c r="E24" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="22" t="s">
-        <v>59</v>
       </c>
       <c r="B25" s="24" t="s">
         <v>43</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="29" t="s">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="B26" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="D26" s="1"/>
+      <c r="E26" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="B26" s="25" t="s">
+      <c r="B27" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="C26" s="21" t="s">
+      <c r="C27" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="D26" s="3"/>
-      <c r="E26" s="11"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added filter API on services
</commit_message>
<xml_diff>
--- a/API_endpoint_list.xlsx
+++ b/API_endpoint_list.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Technikus\Documents\GitHub\HandyGo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Munka\13C_info2\HandyGo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EABEF09-69A2-4D12-8CDC-0B2A46BBD25F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A495160-372B-46DD-94DA-FFD3EA998441}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E0E4588E-4664-4B85-8DE9-D10EECA0DBCE}"/>
+    <workbookView xWindow="1860" yWindow="1860" windowWidth="21600" windowHeight="11295" xr2:uid="{E0E4588E-4664-4B85-8DE9-D10EECA0DBCE}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -243,16 +243,16 @@
     <t>paraméter adatok</t>
   </si>
   <si>
-    <t>service/:lat/:lon</t>
-  </si>
-  <si>
-    <t>szélesség, hosszúság</t>
-  </si>
-  <si>
     <t>service/my-services</t>
   </si>
   <si>
     <t>A felhasználó szolgáltatásainak lekérése</t>
+  </si>
+  <si>
+    <t>service/:lat/:lon/:distance</t>
+  </si>
+  <si>
+    <t>szélesség, hosszúság, távolság</t>
   </si>
 </sst>
 </file>
@@ -1004,7 +1004,7 @@
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1147,7 +1147,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>44</v>
@@ -1157,7 +1157,7 @@
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="10" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1222,13 +1222,13 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="26" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B14" s="16" t="s">
         <v>44</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D14" s="16"/>
       <c r="E14" s="17"/>

</xml_diff>

<commit_message>
Add service creator and responsive filters
Introduce a ServiceCreator component (HTML, TS, spec and CSS) and register it in app.module and routes (path: my-services/service-creator, guarded by auth/verified). The new component provides a form to create services, validates inputs (allows price >= 0), calls service.createService and navigates to /my-services on success.

Update main page UI to a responsive filter drawer: add toggle button, drawer CSS, and open/close behavior; adjust MainComponent to track filterOpen and set priceRange min to 0 (resetFilters updated accordingly).

Backend: relax service creation validation in serviceController.js to accept price === 0 and add a console.log(req.body) for debugging.

Other: small changes to MyServices (import UsersService and an empty-state message in the template) and a binary update to API_endpoint_list.xlsx.
</commit_message>
<xml_diff>
--- a/API_endpoint_list.xlsx
+++ b/API_endpoint_list.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Munka\13C_info2\HandyGo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Technikus\Documents\GitHub\HandyGo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A495160-372B-46DD-94DA-FFD3EA998441}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54EC6838-F73D-41FB-B70F-E95A1178C893}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="1860" windowWidth="21600" windowHeight="11295" xr2:uid="{E0E4588E-4664-4B85-8DE9-D10EECA0DBCE}"/>
+    <workbookView xWindow="135" yWindow="1530" windowWidth="23130" windowHeight="11295" xr2:uid="{E0E4588E-4664-4B85-8DE9-D10EECA0DBCE}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -1004,7 +1004,7 @@
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1013,7 +1013,7 @@
     <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="41.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Fix auth status codes, service model, add tests
Add dotenv loading and improve error handling across auth and admin controllers (use 404 for missing user/email, 401 for invalid password, and 500 for unexpected errors). Return a proper 201 JSON response on admin registration. In serviceController, return 404 when a requested service is not found. Fix Service model create method to query and return the actual inserted service id instead of an incorrect value. Add jest.config.js and update package.json to include Jest and Supertest for tests; update/ add backend test files and API endpoint spreadsheet.
</commit_message>
<xml_diff>
--- a/API_endpoint_list.xlsx
+++ b/API_endpoint_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Munka\13C_info2\HandyGo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E193EC0F-9944-4154-92A8-A0BB79E4641D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB4CAA12-3515-42C0-8DB8-28D5A5CD298A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E0E4588E-4664-4B85-8DE9-D10EECA0DBCE}"/>
   </bookViews>
@@ -1032,7 +1032,7 @@
   <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>